<commit_message>
Changes to excel template
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Desktop\Computer Science\git_practice2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58630A2-96C3-4D58-9777-E32A9D9B5598}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3B1354-5F46-460D-9956-7938731DA8B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5040" yWindow="3840" windowWidth="20700" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,7 +345,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>